<commit_message>
More data and text fixes, as requested.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_naplan_uploader/education_naplan.xlsx
+++ b/dashboard_loader/education_naplan_uploader/education_naplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Mean reading" sheetId="1" state="visible" r:id="rId2"/>
@@ -132,7 +132,7 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">The National Assessment Program—Literacy and Numeracy (NAPLAN) measures proportions of children in Years 3, 5, 7 and 9 meeting national minimum standards (NMS) and their average scores. Tracking these measures over time provides an indication of the performance of students, schools, jurisdictions and the system as a whole. Results for the Northern Territory may reflect, in part, a high proportion of disadvantaged Indigenous students. In the Northern Territory, Indigenous children made up 44 per cent of the 5–19 year old population.</t>
+    <t xml:space="preserve">The National Assessment Program—Literacy and Numeracy (NAPLAN) measures proportions of children in Years 3, 5, 7 and 9 meeting national minimum standards (NMS) and their average scores. Tracking these measures over time provides an indication of the performance of students, schools, jurisdictions and the system as a whole. Results for the Northern Territory may reflect, in part, a high proportion of disadvantaged Indigenous students, smaller test populations and higher volatility in results. In the Northern Territory, Indigenous children made up 44 per cent of the 5–19 year old population.</t>
   </si>
   <si>
     <t xml:space="preserve">Nationally, between 2008 and 2017, at the national level, four areas showed improvements in the proportion of students at or above the national minimum standard. The four areas with significant improvement were Year 3 and 5 reading, and Years 5 and 9 numeracy.</t>
@@ -270,11 +270,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -288,10 +284,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,7 +318,7 @@
   </sheetPr>
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2357,7 +2349,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B55" s="0" t="s">
@@ -2395,7 +2387,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B56" s="0" t="s">
@@ -2433,7 +2425,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B57" s="0" t="s">
@@ -2442,36 +2434,36 @@
       <c r="C57" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="2" t="n">
+      <c r="D57" s="1" t="n">
         <v>0.246079139051119</v>
       </c>
-      <c r="E57" s="2" t="n">
+      <c r="E57" s="1" t="n">
         <v>0.241041298409127</v>
       </c>
-      <c r="F57" s="2" t="n">
+      <c r="F57" s="1" t="n">
         <v>0.300190681120648</v>
       </c>
-      <c r="G57" s="2" t="n">
+      <c r="G57" s="1" t="n">
         <v>0.388912115584681</v>
       </c>
-      <c r="H57" s="2" t="n">
+      <c r="H57" s="1" t="n">
         <v>0.440781064045489</v>
       </c>
-      <c r="I57" s="2" t="n">
+      <c r="I57" s="1" t="n">
         <v>0.721816668190502</v>
       </c>
-      <c r="J57" s="2" t="n">
+      <c r="J57" s="1" t="n">
         <v>0.781921964187974</v>
       </c>
-      <c r="K57" s="2" t="n">
+      <c r="K57" s="1" t="n">
         <v>3.0090868464174</v>
       </c>
-      <c r="L57" s="2" t="n">
+      <c r="L57" s="1" t="n">
         <v>0.141953373048733</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B58" s="0" t="s">
@@ -2509,7 +2501,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B59" s="0" t="s">
@@ -2547,7 +2539,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B60" s="0" t="s">
@@ -2556,36 +2548,36 @@
       <c r="C60" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="2" t="n">
+      <c r="D60" s="1" t="n">
         <v>0.210911136107986</v>
       </c>
-      <c r="E60" s="2" t="n">
+      <c r="E60" s="1" t="n">
         <v>0.178462368235285</v>
       </c>
-      <c r="F60" s="2" t="n">
+      <c r="F60" s="1" t="n">
         <v>0.223239653856769</v>
       </c>
-      <c r="G60" s="2" t="n">
+      <c r="G60" s="1" t="n">
         <v>0.306797403266779</v>
       </c>
-      <c r="H60" s="2" t="n">
+      <c r="H60" s="1" t="n">
         <v>0.350939485646575</v>
       </c>
-      <c r="I60" s="2" t="n">
+      <c r="I60" s="1" t="n">
         <v>0.6644613365282</v>
       </c>
-      <c r="J60" s="2" t="n">
+      <c r="J60" s="1" t="n">
         <v>0.588697017268446</v>
       </c>
-      <c r="K60" s="2" t="n">
+      <c r="K60" s="1" t="n">
         <v>2.02942307418431</v>
       </c>
-      <c r="L60" s="2" t="n">
+      <c r="L60" s="1" t="n">
         <v>0.110979729048036</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B61" s="0" t="s">
@@ -2623,7 +2615,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B62" s="0" t="s">
@@ -2661,7 +2653,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B63" s="0" t="s">
@@ -2670,36 +2662,36 @@
       <c r="C63" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="2" t="n">
+      <c r="D63" s="1" t="n">
         <v>0.279512827775376</v>
       </c>
-      <c r="E63" s="2" t="n">
+      <c r="E63" s="1" t="n">
         <v>0.24088080847011</v>
       </c>
-      <c r="F63" s="2" t="n">
+      <c r="F63" s="1" t="n">
         <v>0.321120673371163</v>
       </c>
-      <c r="G63" s="2" t="n">
+      <c r="G63" s="1" t="n">
         <v>0.492584705623802</v>
       </c>
-      <c r="H63" s="2" t="n">
+      <c r="H63" s="1" t="n">
         <v>0.30117193529321</v>
       </c>
-      <c r="I63" s="2" t="n">
+      <c r="I63" s="1" t="n">
         <v>0.754879351407661</v>
       </c>
-      <c r="J63" s="2" t="n">
+      <c r="J63" s="1" t="n">
         <v>0.781156329364575</v>
       </c>
-      <c r="K63" s="2" t="n">
+      <c r="K63" s="1" t="n">
         <v>2.57853194142956</v>
       </c>
-      <c r="L63" s="2" t="n">
+      <c r="L63" s="1" t="n">
         <v>0.140500481448316</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B64" s="0" t="s">
@@ -2737,7 +2729,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B65" s="0" t="s">
@@ -2775,7 +2767,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B66" s="0" t="s">
@@ -2784,31 +2776,31 @@
       <c r="C66" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D66" s="2" t="n">
+      <c r="D66" s="1" t="n">
         <v>0.243161094224924</v>
       </c>
-      <c r="E66" s="2" t="n">
+      <c r="E66" s="1" t="n">
         <v>0.245290423861852</v>
       </c>
-      <c r="F66" s="2" t="n">
+      <c r="F66" s="1" t="n">
         <v>0.283989052222037</v>
       </c>
-      <c r="G66" s="2" t="n">
+      <c r="G66" s="1" t="n">
         <v>0.420425681002015</v>
       </c>
-      <c r="H66" s="2" t="n">
+      <c r="H66" s="1" t="n">
         <v>0.446841900186244</v>
       </c>
-      <c r="I66" s="2" t="n">
+      <c r="I66" s="1" t="n">
         <v>0.652961044165212</v>
       </c>
-      <c r="J66" s="2" t="n">
+      <c r="J66" s="1" t="n">
         <v>0.676390710672589</v>
       </c>
-      <c r="K66" s="2" t="n">
+      <c r="K66" s="1" t="n">
         <v>2.28759982253771</v>
       </c>
-      <c r="L66" s="2" t="n">
+      <c r="L66" s="1" t="n">
         <v>0.131744899715782</v>
       </c>
     </row>
@@ -4861,7 +4853,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B55" s="0" t="s">
@@ -4899,7 +4891,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B56" s="0" t="s">
@@ -4937,7 +4929,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B57" s="0" t="s">
@@ -4946,36 +4938,36 @@
       <c r="C57" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="2" t="n">
+      <c r="D57" s="1" t="n">
         <v>0.160273533497168</v>
       </c>
-      <c r="E57" s="2" t="n">
+      <c r="E57" s="1" t="n">
         <v>0.213028844105492</v>
       </c>
-      <c r="F57" s="2" t="n">
+      <c r="F57" s="1" t="n">
         <v>0.213698044662891</v>
       </c>
-      <c r="G57" s="2" t="n">
+      <c r="G57" s="1" t="n">
         <v>0.326008997848341</v>
       </c>
-      <c r="H57" s="2" t="n">
+      <c r="H57" s="1" t="n">
         <v>0.438413818803569</v>
       </c>
-      <c r="I57" s="2" t="n">
+      <c r="I57" s="1" t="n">
         <v>0.486423382912487</v>
       </c>
-      <c r="J57" s="2" t="n">
+      <c r="J57" s="1" t="n">
         <v>0.587054905644266</v>
       </c>
-      <c r="K57" s="2" t="n">
+      <c r="K57" s="1" t="n">
         <v>4.32857426698078</v>
       </c>
-      <c r="L57" s="2" t="n">
+      <c r="L57" s="1" t="n">
         <v>0.1075245693641</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B58" s="0" t="s">
@@ -5013,7 +5005,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B59" s="0" t="s">
@@ -5051,7 +5043,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B60" s="0" t="s">
@@ -5060,36 +5052,36 @@
       <c r="C60" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="2" t="n">
+      <c r="D60" s="1" t="n">
         <v>0.162313069448352</v>
       </c>
-      <c r="E60" s="2" t="n">
+      <c r="E60" s="1" t="n">
         <v>0.214371462870863</v>
       </c>
-      <c r="F60" s="2" t="n">
+      <c r="F60" s="1" t="n">
         <v>0.216417425931136</v>
       </c>
-      <c r="G60" s="2" t="n">
+      <c r="G60" s="1" t="n">
         <v>0.384024577572965</v>
       </c>
-      <c r="H60" s="2" t="n">
+      <c r="H60" s="1" t="n">
         <v>0.49857076381041</v>
       </c>
-      <c r="I60" s="2" t="n">
+      <c r="I60" s="1" t="n">
         <v>0.718597298074159</v>
       </c>
-      <c r="J60" s="2" t="n">
+      <c r="J60" s="1" t="n">
         <v>0.587054905644266</v>
       </c>
-      <c r="K60" s="2" t="n">
+      <c r="K60" s="1" t="n">
         <v>4.98304277979413</v>
       </c>
-      <c r="L60" s="2" t="n">
+      <c r="L60" s="1" t="n">
         <v>0.108669665949447</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B61" s="0" t="s">
@@ -5127,7 +5119,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B62" s="0" t="s">
@@ -5165,7 +5157,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B63" s="0" t="s">
@@ -5174,36 +5166,36 @@
       <c r="C63" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="2" t="n">
+      <c r="D63" s="1" t="n">
         <v>0.269949249541086</v>
       </c>
-      <c r="E63" s="2" t="n">
+      <c r="E63" s="1" t="n">
         <v>0.322573708092299</v>
       </c>
-      <c r="F63" s="2" t="n">
+      <c r="F63" s="1" t="n">
         <v>0.326008997848341</v>
       </c>
-      <c r="G63" s="2" t="n">
+      <c r="G63" s="1" t="n">
         <v>0.54919707387799</v>
       </c>
-      <c r="H63" s="2" t="n">
+      <c r="H63" s="1" t="n">
         <v>0.43560647311219</v>
       </c>
-      <c r="I63" s="2" t="n">
+      <c r="I63" s="1" t="n">
         <v>0.822025910256691</v>
       </c>
-      <c r="J63" s="2" t="n">
+      <c r="J63" s="1" t="n">
         <v>0.742500742500743</v>
       </c>
-      <c r="K63" s="2" t="n">
+      <c r="K63" s="1" t="n">
         <v>7.66072194643623</v>
       </c>
-      <c r="L63" s="2" t="n">
+      <c r="L63" s="1" t="n">
         <v>0.162831089882762</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B64" s="0" t="s">
@@ -5241,7 +5233,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B65" s="0" t="s">
@@ -5279,7 +5271,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B66" s="0" t="s">
@@ -5288,31 +5280,31 @@
       <c r="C66" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D66" s="2" t="n">
+      <c r="D66" s="1" t="n">
         <v>0.328457563282824</v>
       </c>
-      <c r="E66" s="2" t="n">
+      <c r="E66" s="1" t="n">
         <v>0.388198757763975</v>
       </c>
-      <c r="F66" s="2" t="n">
+      <c r="F66" s="1" t="n">
         <v>0.44951901465432</v>
       </c>
-      <c r="G66" s="2" t="n">
+      <c r="G66" s="1" t="n">
         <v>0.605420161592145</v>
       </c>
-      <c r="H66" s="2" t="n">
+      <c r="H66" s="1" t="n">
         <v>1.25976316452507</v>
       </c>
-      <c r="I66" s="2" t="n">
+      <c r="I66" s="1" t="n">
         <v>1.1504037917309</v>
       </c>
-      <c r="J66" s="2" t="n">
+      <c r="J66" s="1" t="n">
         <v>0.869357327595575</v>
       </c>
-      <c r="K66" s="2" t="n">
+      <c r="K66" s="1" t="n">
         <v>7.6997262319562</v>
       </c>
-      <c r="L66" s="2" t="n">
+      <c r="L66" s="1" t="n">
         <v>0.222553579774331</v>
       </c>
     </row>
@@ -7076,7 +7068,7 @@
       <c r="E47" s="0" t="n">
         <v>1.8</v>
       </c>
-      <c r="F47" s="1" t="n">
+      <c r="F47" s="0" t="n">
         <v>2.1</v>
       </c>
       <c r="G47" s="0" t="n">
@@ -7365,7 +7357,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
+      <c r="A55" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B55" s="0" t="s">
@@ -7403,7 +7395,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
+      <c r="A56" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B56" s="0" t="s">
@@ -7441,7 +7433,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
+      <c r="A57" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B57" s="0" t="s">
@@ -7450,36 +7442,36 @@
       <c r="C57" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="2" t="n">
+      <c r="D57" s="1" t="n">
         <v>0.233643710557252</v>
       </c>
-      <c r="E57" s="2" t="n">
+      <c r="E57" s="1" t="n">
         <v>0.230751667484418</v>
       </c>
-      <c r="F57" s="2" t="n">
+      <c r="F57" s="1" t="n">
         <v>0.27907731963994</v>
       </c>
-      <c r="G57" s="2" t="n">
+      <c r="G57" s="1" t="n">
         <v>0.342418846733324</v>
       </c>
-      <c r="H57" s="2" t="n">
+      <c r="H57" s="1" t="n">
         <v>0.430937668130984</v>
       </c>
-      <c r="I57" s="2" t="n">
+      <c r="I57" s="1" t="n">
         <v>0.596804177121321</v>
       </c>
-      <c r="J57" s="2" t="n">
+      <c r="J57" s="1" t="n">
         <v>0.707769355051277</v>
       </c>
-      <c r="K57" s="2" t="n">
+      <c r="K57" s="1" t="n">
         <v>2.07788946226015</v>
       </c>
-      <c r="L57" s="2" t="n">
+      <c r="L57" s="1" t="n">
         <v>0.124622394145738</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+      <c r="A58" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B58" s="0" t="s">
@@ -7517,7 +7509,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="n">
+      <c r="A59" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B59" s="0" t="s">
@@ -7555,7 +7547,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
+      <c r="A60" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B60" s="0" t="s">
@@ -7564,36 +7556,36 @@
       <c r="C60" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="2" t="n">
+      <c r="D60" s="1" t="n">
         <v>0.194538983564528</v>
       </c>
-      <c r="E60" s="2" t="n">
+      <c r="E60" s="1" t="n">
         <v>0.162712085033336</v>
       </c>
-      <c r="F60" s="2" t="n">
+      <c r="F60" s="1" t="n">
         <v>0.197672870126844</v>
       </c>
-      <c r="G60" s="2" t="n">
+      <c r="G60" s="1" t="n">
         <v>0.281938399592338</v>
       </c>
-      <c r="H60" s="2" t="n">
+      <c r="H60" s="1" t="n">
         <v>0.310186967868909</v>
       </c>
-      <c r="I60" s="2" t="n">
+      <c r="I60" s="1" t="n">
         <v>0.551228178784499</v>
       </c>
-      <c r="J60" s="2" t="n">
+      <c r="J60" s="1" t="n">
         <v>0.502512562814071</v>
       </c>
-      <c r="K60" s="2" t="n">
+      <c r="K60" s="1" t="n">
         <v>1.39329047981146</v>
       </c>
-      <c r="L60" s="2" t="n">
+      <c r="L60" s="1" t="n">
         <v>0.103322009241121</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
+      <c r="A61" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B61" s="0" t="s">
@@ -7631,7 +7623,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="n">
+      <c r="A62" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B62" s="0" t="s">
@@ -7669,7 +7661,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="n">
+      <c r="A63" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B63" s="0" t="s">
@@ -7678,36 +7670,36 @@
       <c r="C63" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="2" t="n">
+      <c r="D63" s="1" t="n">
         <v>0.328928132857728</v>
       </c>
-      <c r="E63" s="2" t="n">
+      <c r="E63" s="1" t="n">
         <v>0.273470117008747</v>
       </c>
-      <c r="F63" s="2" t="n">
+      <c r="F63" s="1" t="n">
         <v>0.334377333675141</v>
       </c>
-      <c r="G63" s="2" t="n">
+      <c r="G63" s="1" t="n">
         <v>0.536764678663049</v>
       </c>
-      <c r="H63" s="2" t="n">
+      <c r="H63" s="1" t="n">
         <v>0.328256302521008</v>
       </c>
-      <c r="I63" s="2" t="n">
+      <c r="I63" s="1" t="n">
         <v>0.710063205092763</v>
       </c>
-      <c r="J63" s="2" t="n">
+      <c r="J63" s="1" t="n">
         <v>0.776496811795443</v>
       </c>
-      <c r="K63" s="2" t="n">
+      <c r="K63" s="1" t="n">
         <v>2.07629063895497</v>
       </c>
-      <c r="L63" s="2" t="n">
+      <c r="L63" s="1" t="n">
         <v>0.156589084451257</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="n">
+      <c r="A64" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B64" s="0" t="s">
@@ -7745,7 +7737,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="n">
+      <c r="A65" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B65" s="0" t="s">
@@ -7783,7 +7775,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="n">
+      <c r="A66" s="0" t="n">
         <v>2017</v>
       </c>
       <c r="B66" s="0" t="s">
@@ -7792,31 +7784,31 @@
       <c r="C66" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="D66" s="2" t="n">
+      <c r="D66" s="1" t="n">
         <v>0.280612244897959</v>
       </c>
-      <c r="E66" s="2" t="n">
+      <c r="E66" s="1" t="n">
         <v>0.283781134230196</v>
       </c>
-      <c r="F66" s="2" t="n">
+      <c r="F66" s="1" t="n">
         <v>0.279085993371708</v>
       </c>
-      <c r="G66" s="2" t="n">
+      <c r="G66" s="1" t="n">
         <v>0.445667936248916</v>
       </c>
-      <c r="H66" s="2" t="n">
+      <c r="H66" s="1" t="n">
         <v>0.467672368151688</v>
       </c>
-      <c r="I66" s="2" t="n">
+      <c r="I66" s="1" t="n">
         <v>0.587464574105986</v>
       </c>
-      <c r="J66" s="2" t="n">
+      <c r="J66" s="1" t="n">
         <v>0.744885972512851</v>
       </c>
-      <c r="K66" s="2" t="n">
+      <c r="K66" s="1" t="n">
         <v>1.38504155124654</v>
       </c>
-      <c r="L66" s="2" t="n">
+      <c r="L66" s="1" t="n">
         <v>0.14653605993842</v>
       </c>
     </row>
@@ -7893,2434 +7885,2434 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="3" t="n">
         <v>96.9</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="3" t="n">
         <v>96.5</v>
       </c>
-      <c r="F3" s="4" t="n">
+      <c r="F3" s="3" t="n">
         <v>92</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="3" t="n">
         <v>94.5</v>
       </c>
-      <c r="H3" s="4" t="n">
+      <c r="H3" s="3" t="n">
         <v>93.8</v>
       </c>
-      <c r="I3" s="4" t="n">
+      <c r="I3" s="3" t="n">
         <v>96.7</v>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="J3" s="3" t="n">
         <v>96.4</v>
       </c>
-      <c r="K3" s="4" t="n">
+      <c r="K3" s="3" t="n">
         <v>77</v>
       </c>
-      <c r="L3" s="4" t="n">
+      <c r="L3" s="3" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="3" t="n">
         <v>0.2</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="3" t="n">
         <v>0.2</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="I4" s="4" t="n">
+      <c r="I4" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="K4" s="4" t="n">
+      <c r="K4" s="3" t="n">
         <v>5.6</v>
       </c>
-      <c r="L4" s="4" t="n">
+      <c r="L4" s="3" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="3" t="n">
         <v>0.103199174406605</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="3" t="n">
         <v>0.103626943005181</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="3" t="n">
         <v>0.326086956521739</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="3" t="n">
         <v>0.317460317460317</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="3" t="n">
         <v>0.479744136460554</v>
       </c>
-      <c r="I5" s="4" t="n">
+      <c r="I5" s="3" t="n">
         <v>0.31023784901758</v>
       </c>
-      <c r="J5" s="4" t="n">
+      <c r="J5" s="3" t="n">
         <v>0.622406639004149</v>
       </c>
-      <c r="K5" s="4" t="n">
+      <c r="K5" s="3" t="n">
         <v>3.63636363636364</v>
       </c>
-      <c r="L5" s="4" t="n">
+      <c r="L5" s="3" t="n">
         <v>0.105263157894737</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="3" t="n">
         <v>94.4</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="3" t="n">
         <v>94.6</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="3" t="n">
         <v>90.4</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="3" t="n">
         <v>91.1</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="3" t="n">
         <v>90.5</v>
       </c>
-      <c r="I6" s="4" t="n">
+      <c r="I6" s="3" t="n">
         <v>92.1</v>
       </c>
-      <c r="J6" s="4" t="n">
+      <c r="J6" s="3" t="n">
         <v>94.9</v>
       </c>
-      <c r="K6" s="4" t="n">
+      <c r="K6" s="3" t="n">
         <v>69.1</v>
       </c>
-      <c r="L6" s="4" t="n">
+      <c r="L6" s="3" t="n">
         <v>92.7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="H7" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="4" t="n">
+      <c r="I7" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="K7" s="4" t="n">
+      <c r="K7" s="3" t="n">
         <v>5.9</v>
       </c>
-      <c r="L7" s="4" t="n">
+      <c r="L7" s="3" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="3" t="n">
         <v>0.158898305084746</v>
       </c>
-      <c r="E8" s="4" t="n">
+      <c r="E8" s="3" t="n">
         <v>0.158562367864693</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="3" t="n">
         <v>0.331858407079646</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="3" t="n">
         <v>0.439077936333699</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="3" t="n">
         <v>0.552486187845304</v>
       </c>
-      <c r="I8" s="4" t="n">
+      <c r="I8" s="3" t="n">
         <v>0.651465798045603</v>
       </c>
-      <c r="J8" s="4" t="n">
+      <c r="J8" s="3" t="n">
         <v>0.632244467860906</v>
       </c>
-      <c r="K8" s="4" t="n">
+      <c r="K8" s="3" t="n">
         <v>4.26917510853835</v>
       </c>
-      <c r="L8" s="4" t="n">
+      <c r="L8" s="3" t="n">
         <v>0.107874865156419</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D9" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E9" s="3" t="n">
         <v>96.5</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="3" t="n">
         <v>94.9</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="H9" s="3" t="n">
         <v>94.5</v>
       </c>
-      <c r="I9" s="4" t="n">
+      <c r="I9" s="3" t="n">
         <v>95.2</v>
       </c>
-      <c r="J9" s="4" t="n">
+      <c r="J9" s="3" t="n">
         <v>97.1</v>
       </c>
-      <c r="K9" s="4" t="n">
+      <c r="K9" s="3" t="n">
         <v>75.9</v>
       </c>
-      <c r="L9" s="4" t="n">
+      <c r="L9" s="3" t="n">
         <v>95.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="G10" s="4" t="n">
+      <c r="G10" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="H10" s="4" t="n">
+      <c r="H10" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="I10" s="4" t="n">
+      <c r="I10" s="3" t="n">
         <v>1.3</v>
       </c>
-      <c r="J10" s="4" t="n">
+      <c r="J10" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="K10" s="4" t="n">
+      <c r="K10" s="3" t="n">
         <v>7.2</v>
       </c>
-      <c r="L10" s="4" t="n">
+      <c r="L10" s="3" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="3" t="n">
         <v>0.208333333333333</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="3" t="n">
         <v>0.155440414507772</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="3" t="n">
         <v>0.210748155953635</v>
       </c>
-      <c r="G11" s="4" t="n">
+      <c r="G11" s="3" t="n">
         <v>0.316789862724393</v>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="H11" s="3" t="n">
         <v>0.423280423280423</v>
       </c>
-      <c r="I11" s="4" t="n">
+      <c r="I11" s="3" t="n">
         <v>0.682773109243697</v>
       </c>
-      <c r="J11" s="4" t="n">
+      <c r="J11" s="3" t="n">
         <v>0.617919670442843</v>
       </c>
-      <c r="K11" s="4" t="n">
+      <c r="K11" s="3" t="n">
         <v>4.74308300395257</v>
       </c>
-      <c r="L11" s="4" t="n">
+      <c r="L11" s="3" t="n">
         <v>0.10482180293501</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="3" t="n">
         <v>95.2</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="3" t="n">
         <v>92.4</v>
       </c>
-      <c r="G12" s="4" t="n">
+      <c r="G12" s="3" t="n">
         <v>92.3</v>
       </c>
-      <c r="H12" s="4" t="n">
+      <c r="H12" s="3" t="n">
         <v>92</v>
       </c>
-      <c r="I12" s="4" t="n">
+      <c r="I12" s="3" t="n">
         <v>92.3</v>
       </c>
-      <c r="J12" s="4" t="n">
+      <c r="J12" s="3" t="n">
         <v>96.6</v>
       </c>
-      <c r="K12" s="4" t="n">
+      <c r="K12" s="3" t="n">
         <v>74.1</v>
       </c>
-      <c r="L12" s="4" t="n">
+      <c r="L12" s="3" t="n">
         <v>93.6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="4" t="n">
+      <c r="D13" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="E13" s="4" t="n">
+      <c r="E13" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="G13" s="4" t="n">
+      <c r="G13" s="3" t="n">
         <v>1.1</v>
       </c>
-      <c r="H13" s="4" t="n">
+      <c r="H13" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="I13" s="4" t="n">
+      <c r="I13" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="J13" s="4" t="n">
+      <c r="J13" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="K13" s="4" t="n">
+      <c r="K13" s="3" t="n">
         <v>7.5</v>
       </c>
-      <c r="L13" s="4" t="n">
+      <c r="L13" s="3" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="2" t="n">
         <v>2008</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D14" s="3" t="n">
         <v>0.211193241816262</v>
       </c>
-      <c r="E14" s="4" t="n">
+      <c r="E14" s="3" t="n">
         <v>0.210084033613445</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="3" t="n">
         <v>0.432900432900433</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="3" t="n">
         <v>0.595882990249188</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="3" t="n">
         <v>0.978260869565217</v>
       </c>
-      <c r="I14" s="4" t="n">
+      <c r="I14" s="3" t="n">
         <v>0.975081256771398</v>
       </c>
-      <c r="J14" s="4" t="n">
+      <c r="J14" s="3" t="n">
         <v>0.62111801242236</v>
       </c>
-      <c r="K14" s="4" t="n">
+      <c r="K14" s="3" t="n">
         <v>5.06072874493927</v>
       </c>
-      <c r="L14" s="4" t="n">
+      <c r="L14" s="3" t="n">
         <v>0.16025641025641</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="2" t="n">
         <v>2009</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="4" t="n">
+      <c r="D15" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="E15" s="4" t="n">
+      <c r="E15" s="3" t="n">
         <v>95.6</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="3" t="n">
         <v>92.3</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="3" t="n">
         <v>92.3</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="3" t="n">
         <v>92.7</v>
       </c>
-      <c r="I15" s="4" t="n">
+      <c r="I15" s="3" t="n">
         <v>93.9</v>
       </c>
-      <c r="J15" s="4" t="n">
+      <c r="J15" s="3" t="n">
         <v>94.8</v>
       </c>
-      <c r="K15" s="4" t="n">
+      <c r="K15" s="3" t="n">
         <v>70.4</v>
       </c>
-      <c r="L15" s="4" t="n">
+      <c r="L15" s="3" t="n">
         <v>94</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+      <c r="A16" s="2" t="n">
         <v>2009</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="4" t="n">
+      <c r="D16" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="E16" s="4" t="n">
+      <c r="E16" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="3" t="n">
         <v>92.6</v>
       </c>
-      <c r="G16" s="4" t="n">
+      <c r="G16" s="3" t="n">
         <v>92.8</v>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="H16" s="3" t="n">
         <v>93.3</v>
       </c>
-      <c r="I16" s="4" t="n">
+      <c r="I16" s="3" t="n">
         <v>93.2</v>
       </c>
-      <c r="J16" s="4" t="n">
+      <c r="J16" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="K16" s="4" t="n">
+      <c r="K16" s="3" t="n">
         <v>73.5</v>
       </c>
-      <c r="L16" s="4" t="n">
+      <c r="L16" s="3" t="n">
         <v>94.2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="2" t="n">
         <v>2009</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="4" t="n">
+      <c r="D17" s="3" t="n">
         <v>95.1</v>
       </c>
-      <c r="E17" s="4" t="n">
+      <c r="E17" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="3" t="n">
         <v>94.8</v>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="3" t="n">
         <v>93.6</v>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="3" t="n">
         <v>94.2</v>
       </c>
-      <c r="I17" s="4" t="n">
+      <c r="I17" s="3" t="n">
         <v>93</v>
       </c>
-      <c r="J17" s="4" t="n">
+      <c r="J17" s="3" t="n">
         <v>95.7</v>
       </c>
-      <c r="K17" s="4" t="n">
+      <c r="K17" s="3" t="n">
         <v>74.8</v>
       </c>
-      <c r="L17" s="4" t="n">
+      <c r="L17" s="3" t="n">
         <v>94.8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="2" t="n">
         <v>2009</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="4" t="n">
+      <c r="D18" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="E18" s="4" t="n">
+      <c r="E18" s="3" t="n">
         <v>96.3</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="3" t="n">
         <v>94.5</v>
       </c>
-      <c r="G18" s="4" t="n">
+      <c r="G18" s="3" t="n">
         <v>93.5</v>
       </c>
-      <c r="H18" s="4" t="n">
+      <c r="H18" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="I18" s="4" t="n">
+      <c r="I18" s="3" t="n">
         <v>93.7</v>
       </c>
-      <c r="J18" s="4" t="n">
+      <c r="J18" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="K18" s="4" t="n">
+      <c r="K18" s="3" t="n">
         <v>76.2</v>
       </c>
-      <c r="L18" s="4" t="n">
+      <c r="L18" s="3" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+      <c r="A19" s="2" t="n">
         <v>2010</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="4" t="n">
+      <c r="D19" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E19" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="3" t="n">
         <v>93.4</v>
       </c>
-      <c r="G19" s="4" t="n">
+      <c r="G19" s="3" t="n">
         <v>93.5</v>
       </c>
-      <c r="H19" s="4" t="n">
+      <c r="H19" s="3" t="n">
         <v>93.2</v>
       </c>
-      <c r="I19" s="4" t="n">
+      <c r="I19" s="3" t="n">
         <v>94.6</v>
       </c>
-      <c r="J19" s="4" t="n">
+      <c r="J19" s="3" t="n">
         <v>96.6</v>
       </c>
-      <c r="K19" s="4" t="n">
+      <c r="K19" s="3" t="n">
         <v>72.4</v>
       </c>
-      <c r="L19" s="4" t="n">
+      <c r="L19" s="3" t="n">
         <v>94.3</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+      <c r="A20" s="2" t="n">
         <v>2010</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="4" t="n">
+      <c r="D20" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="3" t="n">
         <v>95.7</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="3" t="n">
         <v>92.6</v>
       </c>
-      <c r="G20" s="4" t="n">
+      <c r="G20" s="3" t="n">
         <v>92.3</v>
       </c>
-      <c r="H20" s="4" t="n">
+      <c r="H20" s="3" t="n">
         <v>92.2</v>
       </c>
-      <c r="I20" s="4" t="n">
+      <c r="I20" s="3" t="n">
         <v>93.2</v>
       </c>
-      <c r="J20" s="4" t="n">
+      <c r="J20" s="3" t="n">
         <v>95.3</v>
       </c>
-      <c r="K20" s="4" t="n">
+      <c r="K20" s="3" t="n">
         <v>69.2</v>
       </c>
-      <c r="L20" s="4" t="n">
+      <c r="L20" s="3" t="n">
         <v>93.7</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="2" t="n">
         <v>2010</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="4" t="n">
+      <c r="D21" s="3" t="n">
         <v>94.9</v>
       </c>
-      <c r="E21" s="4" t="n">
+      <c r="E21" s="3" t="n">
         <v>96.1</v>
       </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="G21" s="4" t="n">
+      <c r="G21" s="3" t="n">
         <v>94.8</v>
       </c>
-      <c r="H21" s="4" t="n">
+      <c r="H21" s="3" t="n">
         <v>95.2</v>
       </c>
-      <c r="I21" s="4" t="n">
+      <c r="I21" s="3" t="n">
         <v>94.2</v>
       </c>
-      <c r="J21" s="4" t="n">
+      <c r="J21" s="3" t="n">
         <v>96.8</v>
       </c>
-      <c r="K21" s="4" t="n">
+      <c r="K21" s="3" t="n">
         <v>72.4</v>
       </c>
-      <c r="L21" s="4" t="n">
+      <c r="L21" s="3" t="n">
         <v>95.1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="2" t="n">
         <v>2010</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="4" t="n">
+      <c r="D22" s="3" t="n">
         <v>93.1</v>
       </c>
-      <c r="E22" s="4" t="n">
+      <c r="E22" s="3" t="n">
         <v>94.8</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="3" t="n">
         <v>93.1</v>
       </c>
-      <c r="G22" s="4" t="n">
+      <c r="G22" s="3" t="n">
         <v>92</v>
       </c>
-      <c r="H22" s="4" t="n">
+      <c r="H22" s="3" t="n">
         <v>92.1</v>
       </c>
-      <c r="I22" s="4" t="n">
+      <c r="I22" s="3" t="n">
         <v>92.4</v>
       </c>
-      <c r="J22" s="4" t="n">
+      <c r="J22" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="K22" s="4" t="n">
+      <c r="K22" s="3" t="n">
         <v>70.5</v>
       </c>
-      <c r="L22" s="4" t="n">
+      <c r="L22" s="3" t="n">
         <v>93.1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+      <c r="A23" s="2" t="n">
         <v>2011</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="4" t="n">
+      <c r="D23" s="3" t="n">
         <v>96.5</v>
       </c>
-      <c r="E23" s="4" t="n">
+      <c r="E23" s="3" t="n">
         <v>96.2</v>
       </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="3" t="n">
         <v>95.2</v>
       </c>
-      <c r="G23" s="4" t="n">
+      <c r="G23" s="3" t="n">
         <v>95.3</v>
       </c>
-      <c r="H23" s="4" t="n">
+      <c r="H23" s="3" t="n">
         <v>94.1</v>
       </c>
-      <c r="I23" s="4" t="n">
+      <c r="I23" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="J23" s="4" t="n">
+      <c r="J23" s="3" t="n">
         <v>96.5</v>
       </c>
-      <c r="K23" s="4" t="n">
+      <c r="K23" s="3" t="n">
         <v>79.1</v>
       </c>
-      <c r="L23" s="4" t="n">
+      <c r="L23" s="3" t="n">
         <v>95.6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="2" t="n">
         <v>2011</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="4" t="n">
+      <c r="D24" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="E24" s="4" t="n">
+      <c r="E24" s="3" t="n">
         <v>95.6</v>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="3" t="n">
         <v>93.4</v>
       </c>
-      <c r="G24" s="4" t="n">
+      <c r="G24" s="3" t="n">
         <v>93.4</v>
       </c>
-      <c r="H24" s="4" t="n">
+      <c r="H24" s="3" t="n">
         <v>93.1</v>
       </c>
-      <c r="I24" s="4" t="n">
+      <c r="I24" s="3" t="n">
         <v>93.9</v>
       </c>
-      <c r="J24" s="4" t="n">
+      <c r="J24" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="K24" s="4" t="n">
+      <c r="K24" s="3" t="n">
         <v>72.5</v>
       </c>
-      <c r="L24" s="4" t="n">
+      <c r="L24" s="3" t="n">
         <v>94.4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="2" t="n">
         <v>2011</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="4" t="n">
+      <c r="D25" s="3" t="n">
         <v>94.4</v>
       </c>
-      <c r="E25" s="4" t="n">
+      <c r="E25" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="F25" s="4" t="n">
+      <c r="F25" s="3" t="n">
         <v>94.6</v>
       </c>
-      <c r="G25" s="4" t="n">
+      <c r="G25" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="H25" s="4" t="n">
+      <c r="H25" s="3" t="n">
         <v>93.9</v>
       </c>
-      <c r="I25" s="4" t="n">
+      <c r="I25" s="3" t="n">
         <v>92.6</v>
       </c>
-      <c r="J25" s="4" t="n">
+      <c r="J25" s="3" t="n">
         <v>95.7</v>
       </c>
-      <c r="K25" s="4" t="n">
+      <c r="K25" s="3" t="n">
         <v>71.7</v>
       </c>
-      <c r="L25" s="4" t="n">
+      <c r="L25" s="3" t="n">
         <v>94.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="2" t="n">
         <v>2011</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="4" t="n">
+      <c r="D26" s="3" t="n">
         <v>93</v>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="3" t="n">
         <v>94.6</v>
       </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="3" t="n">
         <v>92.8</v>
       </c>
-      <c r="G26" s="4" t="n">
+      <c r="G26" s="3" t="n">
         <v>92.1</v>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="3" t="n">
         <v>91.7</v>
       </c>
-      <c r="I26" s="4" t="n">
+      <c r="I26" s="3" t="n">
         <v>90.9</v>
       </c>
-      <c r="J26" s="4" t="n">
+      <c r="J26" s="3" t="n">
         <v>94.6</v>
       </c>
-      <c r="K26" s="4" t="n">
+      <c r="K26" s="3" t="n">
         <v>72.6</v>
       </c>
-      <c r="L26" s="4" t="n">
+      <c r="L26" s="3" t="n">
         <v>93</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+      <c r="A27" s="2" t="n">
         <v>2012</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="4" t="n">
+      <c r="D27" s="3" t="n">
         <v>95.1</v>
       </c>
-      <c r="E27" s="4" t="n">
+      <c r="E27" s="3" t="n">
         <v>95.6</v>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="3" t="n">
         <v>92.7</v>
       </c>
-      <c r="G27" s="4" t="n">
+      <c r="G27" s="3" t="n">
         <v>92.5</v>
       </c>
-      <c r="H27" s="4" t="n">
+      <c r="H27" s="3" t="n">
         <v>91.9</v>
       </c>
-      <c r="I27" s="4" t="n">
+      <c r="I27" s="3" t="n">
         <v>93.9</v>
       </c>
-      <c r="J27" s="4" t="n">
+      <c r="J27" s="3" t="n">
         <v>96.5</v>
       </c>
-      <c r="K27" s="4" t="n">
+      <c r="K27" s="3" t="n">
         <v>70</v>
       </c>
-      <c r="L27" s="4" t="n">
+      <c r="L27" s="3" t="n">
         <v>93.9</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="2" t="n">
         <v>2012</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="4" t="n">
+      <c r="D28" s="3" t="n">
         <v>94.5</v>
       </c>
-      <c r="E28" s="4" t="n">
+      <c r="E28" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="F28" s="4" t="n">
+      <c r="F28" s="3" t="n">
         <v>91.7</v>
       </c>
-      <c r="G28" s="4" t="n">
+      <c r="G28" s="3" t="n">
         <v>91.7</v>
       </c>
-      <c r="H28" s="4" t="n">
+      <c r="H28" s="3" t="n">
         <v>91.7</v>
       </c>
-      <c r="I28" s="4" t="n">
+      <c r="I28" s="3" t="n">
         <v>92.6</v>
       </c>
-      <c r="J28" s="4" t="n">
+      <c r="J28" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="K28" s="4" t="n">
+      <c r="K28" s="3" t="n">
         <v>66.5</v>
       </c>
-      <c r="L28" s="4" t="n">
+      <c r="L28" s="3" t="n">
         <v>93.3</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="2" t="n">
         <v>2012</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="4" t="n">
+      <c r="D29" s="3" t="n">
         <v>93.8</v>
       </c>
-      <c r="E29" s="4" t="n">
+      <c r="E29" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="F29" s="4" t="n">
+      <c r="F29" s="3" t="n">
         <v>93.8</v>
       </c>
-      <c r="G29" s="4" t="n">
+      <c r="G29" s="3" t="n">
         <v>93.9</v>
       </c>
-      <c r="H29" s="4" t="n">
+      <c r="H29" s="3" t="n">
         <v>93.5</v>
       </c>
-      <c r="I29" s="4" t="n">
+      <c r="I29" s="3" t="n">
         <v>93.2</v>
       </c>
-      <c r="J29" s="4" t="n">
+      <c r="J29" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="K29" s="4" t="n">
+      <c r="K29" s="3" t="n">
         <v>70.5</v>
       </c>
-      <c r="L29" s="4" t="n">
+      <c r="L29" s="3" t="n">
         <v>93.8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+      <c r="A30" s="2" t="n">
         <v>2012</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="4" t="n">
+      <c r="D30" s="3" t="n">
         <v>93.7</v>
       </c>
-      <c r="E30" s="4" t="n">
+      <c r="E30" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="F30" s="4" t="n">
+      <c r="F30" s="3" t="n">
         <v>93.7</v>
       </c>
-      <c r="G30" s="4" t="n">
+      <c r="G30" s="3" t="n">
         <v>93.1</v>
       </c>
-      <c r="H30" s="4" t="n">
+      <c r="H30" s="3" t="n">
         <v>92.9</v>
       </c>
-      <c r="I30" s="4" t="n">
+      <c r="I30" s="3" t="n">
         <v>92.4</v>
       </c>
-      <c r="J30" s="4" t="n">
+      <c r="J30" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="K30" s="4" t="n">
+      <c r="K30" s="3" t="n">
         <v>74</v>
       </c>
-      <c r="L30" s="4" t="n">
+      <c r="L30" s="3" t="n">
         <v>93.7</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+      <c r="A31" s="2" t="n">
         <v>2013</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="4" t="n">
+      <c r="D31" s="3" t="n">
         <v>96.4</v>
       </c>
-      <c r="E31" s="4" t="n">
+      <c r="E31" s="3" t="n">
         <v>96.2</v>
       </c>
-      <c r="F31" s="4" t="n">
+      <c r="F31" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="G31" s="4" t="n">
+      <c r="G31" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="H31" s="4" t="n">
+      <c r="H31" s="3" t="n">
         <v>94.4</v>
       </c>
-      <c r="I31" s="4" t="n">
+      <c r="I31" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="J31" s="4" t="n">
+      <c r="J31" s="3" t="n">
         <v>96.6</v>
       </c>
-      <c r="K31" s="4" t="n">
+      <c r="K31" s="3" t="n">
         <v>75.7</v>
       </c>
-      <c r="L31" s="4" t="n">
+      <c r="L31" s="3" t="n">
         <v>95.7</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
+      <c r="A32" s="2" t="n">
         <v>2013</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="4" t="n">
+      <c r="D32" s="3" t="n">
         <v>93.9</v>
       </c>
-      <c r="E32" s="4" t="n">
+      <c r="E32" s="3" t="n">
         <v>94.4</v>
       </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="3" t="n">
         <v>93.6</v>
       </c>
-      <c r="G32" s="4" t="n">
+      <c r="G32" s="3" t="n">
         <v>92.7</v>
       </c>
-      <c r="H32" s="4" t="n">
+      <c r="H32" s="3" t="n">
         <v>92</v>
       </c>
-      <c r="I32" s="4" t="n">
+      <c r="I32" s="3" t="n">
         <v>92.4</v>
       </c>
-      <c r="J32" s="4" t="n">
+      <c r="J32" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="K32" s="4" t="n">
+      <c r="K32" s="3" t="n">
         <v>69.7</v>
       </c>
-      <c r="L32" s="4" t="n">
+      <c r="L32" s="3" t="n">
         <v>93.4</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="n">
+      <c r="A33" s="2" t="n">
         <v>2013</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="4" t="n">
+      <c r="D33" s="3" t="n">
         <v>95.1</v>
       </c>
-      <c r="E33" s="4" t="n">
+      <c r="E33" s="3" t="n">
         <v>95.7</v>
       </c>
-      <c r="F33" s="4" t="n">
+      <c r="F33" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="G33" s="4" t="n">
+      <c r="G33" s="3" t="n">
         <v>95.1</v>
       </c>
-      <c r="H33" s="4" t="n">
+      <c r="H33" s="3" t="n">
         <v>94.6</v>
       </c>
-      <c r="I33" s="4" t="n">
+      <c r="I33" s="3" t="n">
         <v>94.5</v>
       </c>
-      <c r="J33" s="4" t="n">
+      <c r="J33" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="K33" s="4" t="n">
+      <c r="K33" s="3" t="n">
         <v>72.3</v>
       </c>
-      <c r="L33" s="4" t="n">
+      <c r="L33" s="3" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="n">
+      <c r="A34" s="2" t="n">
         <v>2013</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="4" t="n">
+      <c r="D34" s="3" t="n">
         <v>90.4</v>
       </c>
-      <c r="E34" s="4" t="n">
+      <c r="E34" s="3" t="n">
         <v>92.2</v>
       </c>
-      <c r="F34" s="4" t="n">
+      <c r="F34" s="3" t="n">
         <v>90.1</v>
       </c>
-      <c r="G34" s="4" t="n">
+      <c r="G34" s="3" t="n">
         <v>90.8</v>
       </c>
-      <c r="H34" s="4" t="n">
+      <c r="H34" s="3" t="n">
         <v>90.1</v>
       </c>
-      <c r="I34" s="4" t="n">
+      <c r="I34" s="3" t="n">
         <v>88</v>
       </c>
-      <c r="J34" s="4" t="n">
+      <c r="J34" s="3" t="n">
         <v>92.9</v>
       </c>
-      <c r="K34" s="4" t="n">
+      <c r="K34" s="3" t="n">
         <v>68.2</v>
       </c>
-      <c r="L34" s="4" t="n">
+      <c r="L34" s="3" t="n">
         <v>90.6</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="n">
+      <c r="A35" s="2" t="n">
         <v>2014</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="4" t="n">
+      <c r="D35" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="E35" s="4" t="n">
+      <c r="E35" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="F35" s="4" t="n">
+      <c r="F35" s="3" t="n">
         <v>94.6</v>
       </c>
-      <c r="G35" s="4" t="n">
+      <c r="G35" s="3" t="n">
         <v>93.8</v>
       </c>
-      <c r="H35" s="4" t="n">
+      <c r="H35" s="3" t="n">
         <v>93.2</v>
       </c>
-      <c r="I35" s="4" t="n">
+      <c r="I35" s="3" t="n">
         <v>94.5</v>
       </c>
-      <c r="J35" s="4" t="n">
+      <c r="J35" s="3" t="n">
         <v>96.5</v>
       </c>
-      <c r="K35" s="4" t="n">
+      <c r="K35" s="3" t="n">
         <v>73</v>
       </c>
-      <c r="L35" s="4" t="n">
+      <c r="L35" s="3" t="n">
         <v>94.6</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="n">
+      <c r="A36" s="2" t="n">
         <v>2014</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D36" s="4" t="n">
+      <c r="D36" s="3" t="n">
         <v>94.3</v>
       </c>
-      <c r="E36" s="4" t="n">
+      <c r="E36" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="F36" s="4" t="n">
+      <c r="F36" s="3" t="n">
         <v>93.1</v>
       </c>
-      <c r="G36" s="4" t="n">
+      <c r="G36" s="3" t="n">
         <v>92.2</v>
       </c>
-      <c r="H36" s="4" t="n">
+      <c r="H36" s="3" t="n">
         <v>91.8</v>
       </c>
-      <c r="I36" s="4" t="n">
+      <c r="I36" s="3" t="n">
         <v>92.6</v>
       </c>
-      <c r="J36" s="4" t="n">
+      <c r="J36" s="3" t="n">
         <v>95.9</v>
       </c>
-      <c r="K36" s="4" t="n">
+      <c r="K36" s="3" t="n">
         <v>68.2</v>
       </c>
-      <c r="L36" s="4" t="n">
+      <c r="L36" s="3" t="n">
         <v>93.5</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="n">
+      <c r="A37" s="2" t="n">
         <v>2014</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="4" t="n">
+      <c r="D37" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="E37" s="4" t="n">
+      <c r="E37" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="F37" s="4" t="n">
+      <c r="F37" s="3" t="n">
         <v>95.3</v>
       </c>
-      <c r="G37" s="4" t="n">
+      <c r="G37" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="H37" s="4" t="n">
+      <c r="H37" s="3" t="n">
         <v>94.8</v>
       </c>
-      <c r="I37" s="4" t="n">
+      <c r="I37" s="3" t="n">
         <v>94.8</v>
       </c>
-      <c r="J37" s="4" t="n">
+      <c r="J37" s="3" t="n">
         <v>96.3</v>
       </c>
-      <c r="K37" s="4" t="n">
+      <c r="K37" s="3" t="n">
         <v>74.4</v>
       </c>
-      <c r="L37" s="4" t="n">
+      <c r="L37" s="3" t="n">
         <v>95.1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="n">
+      <c r="A38" s="2" t="n">
         <v>2014</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="4" t="n">
+      <c r="D38" s="3" t="n">
         <v>94.5</v>
       </c>
-      <c r="E38" s="4" t="n">
+      <c r="E38" s="3" t="n">
         <v>94.8</v>
       </c>
-      <c r="F38" s="4" t="n">
+      <c r="F38" s="3" t="n">
         <v>94.2</v>
       </c>
-      <c r="G38" s="4" t="n">
+      <c r="G38" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="H38" s="4" t="n">
+      <c r="H38" s="3" t="n">
         <v>92.6</v>
       </c>
-      <c r="I38" s="4" t="n">
+      <c r="I38" s="3" t="n">
         <v>93.5</v>
       </c>
-      <c r="J38" s="4" t="n">
+      <c r="J38" s="3" t="n">
         <v>94.9</v>
       </c>
-      <c r="K38" s="4" t="n">
+      <c r="K38" s="3" t="n">
         <v>74.2</v>
       </c>
-      <c r="L38" s="4" t="n">
+      <c r="L38" s="3" t="n">
         <v>94.1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="n">
+      <c r="A39" s="2" t="n">
         <v>2015</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="4" t="n">
+      <c r="D39" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="E39" s="4" t="n">
+      <c r="E39" s="3" t="n">
         <v>95.3</v>
       </c>
-      <c r="F39" s="4" t="n">
+      <c r="F39" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="G39" s="4" t="n">
+      <c r="G39" s="3" t="n">
         <v>93.7</v>
       </c>
-      <c r="H39" s="4" t="n">
+      <c r="H39" s="3" t="n">
         <v>92.8</v>
       </c>
-      <c r="I39" s="4" t="n">
+      <c r="I39" s="3" t="n">
         <v>94</v>
       </c>
-      <c r="J39" s="4" t="n">
+      <c r="J39" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="K39" s="4" t="n">
+      <c r="K39" s="3" t="n">
         <v>75</v>
       </c>
-      <c r="L39" s="4" t="n">
+      <c r="L39" s="3" t="n">
         <v>94.4</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="n">
+      <c r="A40" s="2" t="n">
         <v>2015</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="4" t="n">
+      <c r="D40" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="E40" s="4" t="n">
+      <c r="E40" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="G40" s="4" t="n">
+      <c r="G40" s="3" t="n">
         <v>94.3</v>
       </c>
-      <c r="H40" s="4" t="n">
+      <c r="H40" s="3" t="n">
         <v>94</v>
       </c>
-      <c r="I40" s="4" t="n">
+      <c r="I40" s="3" t="n">
         <v>94.9</v>
       </c>
-      <c r="J40" s="4" t="n">
+      <c r="J40" s="3" t="n">
         <v>96.5</v>
       </c>
-      <c r="K40" s="4" t="n">
+      <c r="K40" s="3" t="n">
         <v>72.7</v>
       </c>
-      <c r="L40" s="4" t="n">
+      <c r="L40" s="3" t="n">
         <v>95.1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="n">
+      <c r="A41" s="2" t="n">
         <v>2015</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="4" t="n">
+      <c r="D41" s="3" t="n">
         <v>96.1</v>
       </c>
-      <c r="E41" s="4" t="n">
+      <c r="E41" s="3" t="n">
         <v>96.3</v>
       </c>
-      <c r="F41" s="4" t="n">
+      <c r="F41" s="3" t="n">
         <v>96.2</v>
       </c>
-      <c r="G41" s="4" t="n">
+      <c r="G41" s="3" t="n">
         <v>95.6</v>
       </c>
-      <c r="H41" s="4" t="n">
+      <c r="H41" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="I41" s="4" t="n">
+      <c r="I41" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="J41" s="4" t="n">
+      <c r="J41" s="3" t="n">
         <v>96.7</v>
       </c>
-      <c r="K41" s="4" t="n">
+      <c r="K41" s="3" t="n">
         <v>77.4</v>
       </c>
-      <c r="L41" s="4" t="n">
+      <c r="L41" s="3" t="n">
         <v>95.9</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="n">
+      <c r="A42" s="2" t="n">
         <v>2015</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="4" t="n">
+      <c r="D42" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="E42" s="4" t="n">
+      <c r="E42" s="3" t="n">
         <v>95.6</v>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="3" t="n">
         <v>96.3</v>
       </c>
-      <c r="G42" s="4" t="n">
+      <c r="G42" s="3" t="n">
         <v>96.4</v>
       </c>
-      <c r="H42" s="4" t="n">
+      <c r="H42" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="I42" s="4" t="n">
+      <c r="I42" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="J42" s="4" t="n">
+      <c r="J42" s="3" t="n">
         <v>95.2</v>
       </c>
-      <c r="K42" s="4" t="n">
+      <c r="K42" s="3" t="n">
         <v>79.1</v>
       </c>
-      <c r="L42" s="4" t="n">
+      <c r="L42" s="3" t="n">
         <v>95.7</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="n">
+      <c r="A43" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="4" t="n">
+      <c r="D43" s="3" t="n">
         <v>95.9</v>
       </c>
-      <c r="E43" s="4" t="n">
+      <c r="E43" s="3" t="n">
         <v>95.9</v>
       </c>
-      <c r="F43" s="4" t="n">
+      <c r="F43" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="G43" s="4" t="n">
+      <c r="G43" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="H43" s="4" t="n">
+      <c r="H43" s="3" t="n">
         <v>94.2</v>
       </c>
-      <c r="I43" s="4" t="n">
+      <c r="I43" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="J43" s="4" t="n">
+      <c r="J43" s="3" t="n">
         <v>96.9</v>
       </c>
-      <c r="K43" s="4" t="n">
+      <c r="K43" s="3" t="n">
         <v>77.9</v>
       </c>
-      <c r="L43" s="4" t="n">
+      <c r="L43" s="3" t="n">
         <v>95.5</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="n">
+      <c r="A44" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="4" t="n">
+      <c r="D44" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="E44" s="4" t="n">
+      <c r="E44" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="G44" s="4" t="n">
+      <c r="G44" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="H44" s="4" t="n">
+      <c r="H44" s="3" t="n">
         <v>0.7</v>
       </c>
-      <c r="I44" s="4" t="n">
+      <c r="I44" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="J44" s="4" t="n">
+      <c r="J44" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="K44" s="4" t="n">
+      <c r="K44" s="3" t="n">
         <v>5.4</v>
       </c>
-      <c r="L44" s="4" t="n">
+      <c r="L44" s="3" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="n">
+      <c r="A45" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="4" t="n">
+      <c r="D45" s="3" t="n">
         <v>0.156412930135558</v>
       </c>
-      <c r="E45" s="4" t="n">
+      <c r="E45" s="3" t="n">
         <v>0.208550573514077</v>
       </c>
-      <c r="F45" s="4" t="n">
+      <c r="F45" s="3" t="n">
         <v>0.208333333333333</v>
       </c>
-      <c r="G45" s="4" t="n">
+      <c r="G45" s="3" t="n">
         <v>0.263157894736842</v>
       </c>
-      <c r="H45" s="4" t="n">
+      <c r="H45" s="3" t="n">
         <v>0.371549893842887</v>
       </c>
-      <c r="I45" s="4" t="n">
+      <c r="I45" s="3" t="n">
         <v>0.46972860125261</v>
       </c>
-      <c r="J45" s="4" t="n">
+      <c r="J45" s="3" t="n">
         <v>0.412796697626419</v>
       </c>
-      <c r="K45" s="4" t="n">
+      <c r="K45" s="3" t="n">
         <v>3.46598202824133</v>
       </c>
-      <c r="L45" s="4" t="n">
+      <c r="L45" s="3" t="n">
         <v>0.104712041884817</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="n">
+      <c r="A46" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D46" s="4" t="n">
+      <c r="D46" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="E46" s="4" t="n">
+      <c r="E46" s="3" t="n">
         <v>95.3</v>
       </c>
-      <c r="F46" s="4" t="n">
+      <c r="F46" s="3" t="n">
         <v>94.7</v>
       </c>
-      <c r="G46" s="4" t="n">
+      <c r="G46" s="3" t="n">
         <v>93.4</v>
       </c>
-      <c r="H46" s="4" t="n">
+      <c r="H46" s="3" t="n">
         <v>92.8</v>
       </c>
-      <c r="I46" s="4" t="n">
+      <c r="I46" s="3" t="n">
         <v>94</v>
       </c>
-      <c r="J46" s="4" t="n">
+      <c r="J46" s="3" t="n">
         <v>96.3</v>
       </c>
-      <c r="K46" s="4" t="n">
+      <c r="K46" s="3" t="n">
         <v>73.5</v>
       </c>
-      <c r="L46" s="4" t="n">
+      <c r="L46" s="3" t="n">
         <v>94.3</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="n">
+      <c r="A47" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D47" s="4" t="n">
+      <c r="D47" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="E47" s="4" t="n">
+      <c r="E47" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="F47" s="4" t="n">
+      <c r="F47" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="G47" s="4" t="n">
+      <c r="G47" s="3" t="n">
         <v>0.7</v>
       </c>
-      <c r="H47" s="4" t="n">
+      <c r="H47" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="I47" s="4" t="n">
+      <c r="I47" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J47" s="4" t="n">
+      <c r="J47" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="K47" s="4" t="n">
+      <c r="K47" s="3" t="n">
         <v>6.2</v>
       </c>
-      <c r="L47" s="4" t="n">
+      <c r="L47" s="3" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="n">
+      <c r="A48" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="4" t="n">
+      <c r="D48" s="3" t="n">
         <v>0.158394931362196</v>
       </c>
-      <c r="E48" s="4" t="n">
+      <c r="E48" s="3" t="n">
         <v>0.209863588667366</v>
       </c>
-      <c r="F48" s="4" t="n">
+      <c r="F48" s="3" t="n">
         <v>0.263991552270327</v>
       </c>
-      <c r="G48" s="4" t="n">
+      <c r="G48" s="3" t="n">
         <v>0.374732334047109</v>
       </c>
-      <c r="H48" s="4" t="n">
+      <c r="H48" s="3" t="n">
         <v>0.484913793103448</v>
       </c>
-      <c r="I48" s="4" t="n">
+      <c r="I48" s="3" t="n">
         <v>0.531914893617021</v>
       </c>
-      <c r="J48" s="4" t="n">
+      <c r="J48" s="3" t="n">
         <v>0.519210799584631</v>
       </c>
-      <c r="K48" s="4" t="n">
+      <c r="K48" s="3" t="n">
         <v>4.21768707482993</v>
       </c>
-      <c r="L48" s="4" t="n">
+      <c r="L48" s="3" t="n">
         <v>0.106044538706257</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="n">
+      <c r="A49" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="4" t="n">
+      <c r="D49" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="E49" s="4" t="n">
+      <c r="E49" s="3" t="n">
         <v>96.1</v>
       </c>
-      <c r="F49" s="4" t="n">
+      <c r="F49" s="3" t="n">
         <v>95.6</v>
       </c>
-      <c r="G49" s="4" t="n">
+      <c r="G49" s="3" t="n">
         <v>95.1</v>
       </c>
-      <c r="H49" s="4" t="n">
+      <c r="H49" s="3" t="n">
         <v>95.2</v>
       </c>
-      <c r="I49" s="4" t="n">
+      <c r="I49" s="3" t="n">
         <v>95.3</v>
       </c>
-      <c r="J49" s="4" t="n">
+      <c r="J49" s="3" t="n">
         <v>96.7</v>
       </c>
-      <c r="K49" s="4" t="n">
+      <c r="K49" s="3" t="n">
         <v>74.3</v>
       </c>
-      <c r="L49" s="4" t="n">
+      <c r="L49" s="3" t="n">
         <v>95.5</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="3" t="n">
+      <c r="A50" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="4" t="n">
+      <c r="D50" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="E50" s="4" t="n">
+      <c r="E50" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="F50" s="4" t="n">
+      <c r="F50" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="G50" s="4" t="n">
+      <c r="G50" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="H50" s="4" t="n">
+      <c r="H50" s="3" t="n">
         <v>0.7</v>
       </c>
-      <c r="I50" s="4" t="n">
+      <c r="I50" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="J50" s="4" t="n">
+      <c r="J50" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="K50" s="4" t="n">
+      <c r="K50" s="3" t="n">
         <v>8.2</v>
       </c>
-      <c r="L50" s="4" t="n">
+      <c r="L50" s="3" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3" t="n">
+      <c r="A51" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="4" t="n">
+      <c r="D51" s="3" t="n">
         <v>0.208768267223382</v>
       </c>
-      <c r="E51" s="4" t="n">
+      <c r="E51" s="3" t="n">
         <v>0.260145681581686</v>
       </c>
-      <c r="F51" s="4" t="n">
+      <c r="F51" s="3" t="n">
         <v>0.313807531380753</v>
       </c>
-      <c r="G51" s="4" t="n">
+      <c r="G51" s="3" t="n">
         <v>0.420609884332282</v>
       </c>
-      <c r="H51" s="4" t="n">
+      <c r="H51" s="3" t="n">
         <v>0.367647058823529</v>
       </c>
-      <c r="I51" s="4" t="n">
+      <c r="I51" s="3" t="n">
         <v>0.629590766002099</v>
       </c>
-      <c r="J51" s="4" t="n">
+      <c r="J51" s="3" t="n">
         <v>0.62047569803516</v>
       </c>
-      <c r="K51" s="4" t="n">
+      <c r="K51" s="3" t="n">
         <v>5.51816958277254</v>
       </c>
-      <c r="L51" s="4" t="n">
+      <c r="L51" s="3" t="n">
         <v>0.104712041884817</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="3" t="n">
+      <c r="A52" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="4" t="n">
+      <c r="D52" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="E52" s="4" t="n">
+      <c r="E52" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="F52" s="4" t="n">
+      <c r="F52" s="3" t="n">
         <v>95.3</v>
       </c>
-      <c r="G52" s="4" t="n">
+      <c r="G52" s="3" t="n">
         <v>95.9</v>
       </c>
-      <c r="H52" s="4" t="n">
+      <c r="H52" s="3" t="n">
         <v>94.4</v>
       </c>
-      <c r="I52" s="4" t="n">
+      <c r="I52" s="3" t="n">
         <v>95.7</v>
       </c>
-      <c r="J52" s="4" t="n">
+      <c r="J52" s="3" t="n">
         <v>96.4</v>
       </c>
-      <c r="K52" s="4" t="n">
+      <c r="K52" s="3" t="n">
         <v>75.2</v>
       </c>
-      <c r="L52" s="4" t="n">
+      <c r="L52" s="3" t="n">
         <v>95.2</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="n">
+      <c r="A53" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D53" s="4" t="n">
+      <c r="D53" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="E53" s="4" t="n">
+      <c r="E53" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="F53" s="4" t="n">
+      <c r="F53" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="G53" s="4" t="n">
+      <c r="G53" s="3" t="n">
         <v>0.7</v>
       </c>
-      <c r="H53" s="4" t="n">
+      <c r="H53" s="3" t="n">
         <v>1.4</v>
       </c>
-      <c r="I53" s="4" t="n">
+      <c r="I53" s="3" t="n">
         <v>1.1</v>
       </c>
-      <c r="J53" s="4" t="n">
+      <c r="J53" s="3" t="n">
         <v>1.6</v>
       </c>
-      <c r="K53" s="4" t="n">
+      <c r="K53" s="3" t="n">
         <v>8.4</v>
       </c>
-      <c r="L53" s="4" t="n">
+      <c r="L53" s="3" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="3" t="n">
+      <c r="A54" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D54" s="4" t="n">
+      <c r="D54" s="3" t="n">
         <v>0.209643605870021</v>
       </c>
-      <c r="E54" s="4" t="n">
+      <c r="E54" s="3" t="n">
         <v>0.314465408805031</v>
       </c>
-      <c r="F54" s="4" t="n">
+      <c r="F54" s="3" t="n">
         <v>0.314795383001049</v>
       </c>
-      <c r="G54" s="4" t="n">
+      <c r="G54" s="3" t="n">
         <v>0.364963503649635</v>
       </c>
-      <c r="H54" s="4" t="n">
+      <c r="H54" s="3" t="n">
         <v>0.741525423728813</v>
       </c>
-      <c r="I54" s="4" t="n">
+      <c r="I54" s="3" t="n">
         <v>0.574712643678161</v>
       </c>
-      <c r="J54" s="4" t="n">
+      <c r="J54" s="3" t="n">
         <v>0.829875518672199</v>
       </c>
-      <c r="K54" s="4" t="n">
+      <c r="K54" s="3" t="n">
         <v>5.58510638297872</v>
       </c>
-      <c r="L54" s="4" t="n">
+      <c r="L54" s="3" t="n">
         <v>0.157563025210084</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="n">
+      <c r="A55" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="4" t="n">
+      <c r="D55" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="E55" s="4" t="n">
+      <c r="E55" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="F55" s="4" t="n">
+      <c r="F55" s="3" t="n">
         <v>95.7</v>
       </c>
-      <c r="G55" s="4" t="n">
+      <c r="G55" s="3" t="n">
         <v>95.1</v>
       </c>
-      <c r="H55" s="4" t="n">
+      <c r="H55" s="3" t="n">
         <v>93</v>
       </c>
-      <c r="I55" s="4" t="n">
+      <c r="I55" s="3" t="n">
         <v>96.2</v>
       </c>
-      <c r="J55" s="4" t="n">
+      <c r="J55" s="3" t="n">
         <v>96.7</v>
       </c>
-      <c r="K55" s="4" t="n">
+      <c r="K55" s="3" t="n">
         <v>76.3</v>
       </c>
-      <c r="L55" s="4" t="n">
+      <c r="L55" s="3" t="n">
         <v>95.4</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="n">
+      <c r="A56" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="4" t="n">
+      <c r="D56" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="E56" s="4" t="n">
+      <c r="E56" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="F56" s="4" t="n">
+      <c r="F56" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="G56" s="4" t="n">
+      <c r="G56" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="H56" s="4" t="n">
+      <c r="H56" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="I56" s="4" t="n">
+      <c r="I56" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="J56" s="4" t="n">
+      <c r="J56" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="K56" s="4" t="n">
+      <c r="K56" s="3" t="n">
         <v>5.8</v>
       </c>
-      <c r="L56" s="4" t="n">
+      <c r="L56" s="3" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="n">
+      <c r="A57" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="4" t="n">
+      <c r="D57" s="3" t="n">
         <v>0.159438775510204</v>
       </c>
-      <c r="E57" s="4" t="n">
+      <c r="E57" s="3" t="n">
         <v>0.212585034013605</v>
       </c>
-      <c r="F57" s="4" t="n">
+      <c r="F57" s="3" t="n">
         <v>0.213251444778538</v>
       </c>
-      <c r="G57" s="4" t="n">
+      <c r="G57" s="3" t="n">
         <v>0.26824609970171</v>
       </c>
-      <c r="H57" s="4" t="n">
+      <c r="H57" s="3" t="n">
         <v>0.43888523151196</v>
       </c>
-      <c r="I57" s="4" t="n">
+      <c r="I57" s="3" t="n">
         <v>0.424286138571853</v>
       </c>
-      <c r="J57" s="4" t="n">
+      <c r="J57" s="3" t="n">
         <v>0.527615389485681</v>
       </c>
-      <c r="K57" s="4" t="n">
+      <c r="K57" s="3" t="n">
         <v>3.87835343836093</v>
       </c>
-      <c r="L57" s="4" t="n">
+      <c r="L57" s="3" t="n">
         <v>0.106961023403072</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="n">
+      <c r="A58" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D58" s="4" t="n">
+      <c r="D58" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="E58" s="4" t="n">
+      <c r="E58" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="F58" s="4" t="n">
+      <c r="F58" s="3" t="n">
         <v>95.9</v>
       </c>
-      <c r="G58" s="4" t="n">
+      <c r="G58" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="H58" s="4" t="n">
+      <c r="H58" s="3" t="n">
         <v>93.3</v>
       </c>
-      <c r="I58" s="4" t="n">
+      <c r="I58" s="3" t="n">
         <v>95</v>
       </c>
-      <c r="J58" s="4" t="n">
+      <c r="J58" s="3" t="n">
         <v>96.3</v>
       </c>
-      <c r="K58" s="4" t="n">
+      <c r="K58" s="3" t="n">
         <v>74.5</v>
       </c>
-      <c r="L58" s="4" t="n">
+      <c r="L58" s="3" t="n">
         <v>95.4</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="n">
+      <c r="A59" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="4" t="n">
+      <c r="D59" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="E59" s="4" t="n">
+      <c r="E59" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="F59" s="4" t="n">
+      <c r="F59" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="G59" s="4" t="n">
+      <c r="G59" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="H59" s="4" t="n">
+      <c r="H59" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="I59" s="4" t="n">
+      <c r="I59" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J59" s="4" t="n">
+      <c r="J59" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="K59" s="4" t="n">
+      <c r="K59" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="L59" s="4" t="n">
+      <c r="L59" s="3" t="n">
         <v>0.2</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="n">
+      <c r="A60" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="4" t="n">
+      <c r="D60" s="3" t="n">
         <v>0.159771633079119</v>
       </c>
-      <c r="E60" s="4" t="n">
+      <c r="E60" s="3" t="n">
         <v>0.212585034013605</v>
       </c>
-      <c r="F60" s="4" t="n">
+      <c r="F60" s="3" t="n">
         <v>0.212806707667426</v>
       </c>
-      <c r="G60" s="4" t="n">
+      <c r="G60" s="3" t="n">
         <v>0.322234156820623</v>
       </c>
-      <c r="H60" s="4" t="n">
+      <c r="H60" s="3" t="n">
         <v>0.437474024979767</v>
       </c>
-      <c r="I60" s="4" t="n">
+      <c r="I60" s="3" t="n">
         <v>0.537056928034372</v>
       </c>
-      <c r="J60" s="4" t="n">
+      <c r="J60" s="3" t="n">
         <v>0.529806938351665</v>
       </c>
-      <c r="K60" s="4" t="n">
+      <c r="K60" s="3" t="n">
         <v>4.10902616079989</v>
       </c>
-      <c r="L60" s="4" t="n">
+      <c r="L60" s="3" t="n">
         <v>0.106961023403072</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="n">
+      <c r="A61" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D61" s="4" t="n">
+      <c r="D61" s="3" t="n">
         <v>95.8</v>
       </c>
-      <c r="E61" s="4" t="n">
+      <c r="E61" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="F61" s="4" t="n">
+      <c r="F61" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="G61" s="4" t="n">
+      <c r="G61" s="3" t="n">
         <v>94.9</v>
       </c>
-      <c r="H61" s="4" t="n">
+      <c r="H61" s="3" t="n">
         <v>94.9</v>
       </c>
-      <c r="I61" s="4" t="n">
+      <c r="I61" s="3" t="n">
         <v>94.9</v>
       </c>
-      <c r="J61" s="4" t="n">
+      <c r="J61" s="3" t="n">
         <v>96.9</v>
       </c>
-      <c r="K61" s="4" t="n">
+      <c r="K61" s="3" t="n">
         <v>74.1</v>
       </c>
-      <c r="L61" s="4" t="n">
+      <c r="L61" s="3" t="n">
         <v>95.4</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="n">
+      <c r="A62" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D62" s="4" t="n">
+      <c r="D62" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="E62" s="4" t="n">
+      <c r="E62" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="F62" s="4" t="n">
+      <c r="F62" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="G62" s="4" t="n">
+      <c r="G62" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="H62" s="4" t="n">
+      <c r="H62" s="3" t="n">
         <v>0.7</v>
       </c>
-      <c r="I62" s="4" t="n">
+      <c r="I62" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="J62" s="4" t="n">
+      <c r="J62" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="K62" s="4" t="n">
+      <c r="K62" s="3" t="n">
         <v>8.5</v>
       </c>
-      <c r="L62" s="4" t="n">
+      <c r="L62" s="3" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="n">
+      <c r="A63" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D63" s="4" t="n">
+      <c r="D63" s="3" t="n">
         <v>0.213028844105492</v>
       </c>
-      <c r="E63" s="4" t="n">
+      <c r="E63" s="3" t="n">
         <v>0.265731292517007</v>
       </c>
-      <c r="F63" s="4" t="n">
+      <c r="F63" s="3" t="n">
         <v>0.26740255850768</v>
       </c>
-      <c r="G63" s="4" t="n">
+      <c r="G63" s="3" t="n">
         <v>0.430098277456399</v>
       </c>
-      <c r="H63" s="4" t="n">
+      <c r="H63" s="3" t="n">
         <v>0.376335992774349</v>
       </c>
-      <c r="I63" s="4" t="n">
+      <c r="I63" s="3" t="n">
         <v>0.645147416184598</v>
       </c>
-      <c r="J63" s="4" t="n">
+      <c r="J63" s="3" t="n">
         <v>0.631831680040437</v>
       </c>
-      <c r="K63" s="4" t="n">
+      <c r="K63" s="3" t="n">
         <v>5.85254344652841</v>
       </c>
-      <c r="L63" s="4" t="n">
+      <c r="L63" s="3" t="n">
         <v>0.160441535104608</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="n">
+      <c r="A64" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D64" s="4" t="n">
+      <c r="D64" s="3" t="n">
         <v>96.4</v>
       </c>
-      <c r="E64" s="4" t="n">
+      <c r="E64" s="3" t="n">
         <v>95.5</v>
       </c>
-      <c r="F64" s="4" t="n">
+      <c r="F64" s="3" t="n">
         <v>96</v>
       </c>
-      <c r="G64" s="4" t="n">
+      <c r="G64" s="3" t="n">
         <v>96.4</v>
       </c>
-      <c r="H64" s="4" t="n">
+      <c r="H64" s="3" t="n">
         <v>94.3</v>
       </c>
-      <c r="I64" s="4" t="n">
+      <c r="I64" s="3" t="n">
         <v>95.4</v>
       </c>
-      <c r="J64" s="4" t="n">
+      <c r="J64" s="3" t="n">
         <v>96.2</v>
       </c>
-      <c r="K64" s="4" t="n">
+      <c r="K64" s="3" t="n">
         <v>81.2</v>
       </c>
-      <c r="L64" s="4" t="n">
+      <c r="L64" s="3" t="n">
         <v>95.8</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="n">
+      <c r="A65" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D65" s="4" t="n">
+      <c r="D65" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="E65" s="4" t="n">
+      <c r="E65" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="F65" s="4" t="n">
+      <c r="F65" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="G65" s="4" t="n">
+      <c r="G65" s="3" t="n">
         <v>0.7</v>
       </c>
-      <c r="H65" s="4" t="n">
+      <c r="H65" s="3" t="n">
         <v>1.9</v>
       </c>
-      <c r="I65" s="4" t="n">
+      <c r="I65" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="J65" s="4" t="n">
+      <c r="J65" s="3" t="n">
         <v>1.3</v>
       </c>
-      <c r="K65" s="4" t="n">
+      <c r="K65" s="3" t="n">
         <v>6.7</v>
       </c>
-      <c r="L65" s="4" t="n">
+      <c r="L65" s="3" t="n">
         <v>0.3</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="n">
+      <c r="A66" s="2" t="n">
         <v>2017</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D66" s="4" t="n">
+      <c r="D66" s="3" t="n">
         <v>0.211702938436785</v>
       </c>
-      <c r="E66" s="4" t="n">
+      <c r="E66" s="3" t="n">
         <v>0.320547066994337</v>
       </c>
-      <c r="F66" s="4" t="n">
+      <c r="F66" s="3" t="n">
         <v>0.265731292517007</v>
       </c>
-      <c r="G66" s="4" t="n">
+      <c r="G66" s="3" t="n">
         <v>0.370480142264375</v>
       </c>
-      <c r="H66" s="4" t="n">
+      <c r="H66" s="3" t="n">
         <v>1.0279827731729</v>
       </c>
-      <c r="I66" s="4" t="n">
+      <c r="I66" s="3" t="n">
         <v>0.641766140418431</v>
       </c>
-      <c r="J66" s="4" t="n">
+      <c r="J66" s="3" t="n">
         <v>0.689464975179261</v>
       </c>
-      <c r="K66" s="4" t="n">
+      <c r="K66" s="3" t="n">
         <v>4.20981200361918</v>
       </c>
-      <c r="L66" s="4" t="n">
+      <c r="L66" s="3" t="n">
         <v>0.159771633079119</v>
       </c>
     </row>
@@ -10342,8 +10334,8 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10357,59 +10349,59 @@
       <c r="A1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="4" t="n">
         <v>2017</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="100.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="79.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -10417,7 +10409,7 @@
       <c r="A9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -10425,7 +10417,7 @@
       <c r="A10" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>